<commit_message>
Updated excel formulas Python)
</commit_message>
<xml_diff>
--- a/backend/python/templates/FAAS_Template.xlsx
+++ b/backend/python/templates/FAAS_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Videos\FAAS SYSTEM\backend\python\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31FDD4F-D422-40EF-BBCF-81B7D2907303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C41C3F-505F-46B1-963C-95842D6073AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,28 +28,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -688,109 +666,115 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1210,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B52" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67:G67"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1228,28 +1212,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1272,712 +1256,463 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="35"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="45" t="s">
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="75"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="76"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="66"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="43"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="45" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="78"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="76"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="66"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="42" t="s">
+      <c r="F21" s="33"/>
+      <c r="G21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="35"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="48" t="str" cm="1">
-        <f t="array" ref="E22">_xlfn.IFS(
-    A22="COMMERCIAL", _xlfn.IFS(C22="C-1",1400, C22="C-2",1030, C22="C-3",850, C22="C-4",720, TRUE, ""),
-    A22="RESIDENTIAL", _xlfn.IFS(C22="R-1",760, C22="R-2",610, C22="R-3",470, C22="R-4",280, C22="R-5",200, TRUE, ""),
-    A22="COCONUT LAND", _xlfn.IFS(OR(C22=1,C22="1"),93830, OR(C22=2,C22="2"),84500, OR(C22=3,C22="3"),76130, TRUE, ""),
-    A22="RICE LAND W/ IRRIGATION", _xlfn.IFS(OR(C22=1,C22="1"),188760, OR(C22=2,C22="2"),174390, OR(C22=3,C22="3"),126950, TRUE, ""),
-    A22="RICE LAND W/O IRRIGATION", _xlfn.IFS(OR(C22=1,C22="1"),82450, OR(C22=2,C22="2"),75070, OR(C22=3,C22="3"),52590, TRUE, ""),
-    A22="UPLAND RICE", 28540,
-    A22="ORCHARD", 44100,
-    A22="COGON LAND", 46460,
-    A22="NIPA LAND", 55070,
-    A22="FOREST LAND", 59660,
-    A22="FISHPOND", 218240,
-    TRUE, ""
-)</f>
-        <v/>
-      </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="43" t="str">
-        <f>IFERROR(MROUND(D22*E22,10),"")</f>
-        <v/>
-      </c>
-      <c r="H22" s="35"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="26"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="48" t="str" cm="1">
-        <f t="array" ref="E23">_xlfn.IFS(
-    A23="COMMERCIAL", _xlfn.IFS(C23="C-1",1400, C23="C-2",1030, C23="C-3",850, C23="C-4",720, TRUE, ""),
-    A23="RESIDENTIAL", _xlfn.IFS(C23="R-1",760, C23="R-2",610, C23="R-3",470, C23="R-4",280, C23="R-5",200, TRUE, ""),
-    A23="COCONUT LAND", _xlfn.IFS(OR(C23=1,C23="1"),93830, OR(C23=2,C23="2"),84500, OR(C23=3,C23="3"),76130, TRUE, ""),
-    A23="RICE LAND W/ IRRIGATION", _xlfn.IFS(OR(C23=1,C23="1"),188760, OR(C23=2,C23="2"),174390, OR(C23=3,C23="3"),126950, TRUE, ""),
-    A23="RICE LAND W/O IRRIGATION", _xlfn.IFS(OR(C23=1,C23="1"),82450, OR(C23=2,C23="2"),75070, OR(C23=3,C23="3"),52590, TRUE, ""),
-    A23="UPLAND RICE", 28540,
-    A23="ORCHARD", 44100,
-    A23="COGON LAND", 46460,
-    A23="NIPA LAND", 55070,
-    A23="FOREST LAND", 59660,
-    A23="FISHPOND", 218240,
-    TRUE, ""
-)</f>
-        <v/>
-      </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="43" t="str">
-        <f>IFERROR(MROUND(D23*E23,10),"")</f>
-        <v/>
-      </c>
-      <c r="H23" s="35"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="33"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="26"/>
       <c r="D24" s="28"/>
-      <c r="E24" s="48" t="str" cm="1">
-        <f t="array" ref="E24">_xlfn.IFS(
-    A24="COMMERCIAL", _xlfn.IFS(C24="C-1",1400, C24="C-2",1030, C24="C-3",850, C24="C-4",720, TRUE, ""),
-    A24="RESIDENTIAL", _xlfn.IFS(C24="R-1",760, C24="R-2",610, C24="R-3",470, C24="R-4",280, C24="R-5",200, TRUE, ""),
-    A24="COCONUT LAND", _xlfn.IFS(OR(C24=1,C24="1"),93830, OR(C24=2,C24="2"),84500, OR(C24=3,C24="3"),76130, TRUE, ""),
-    A24="RICE LAND W/ IRRIGATION", _xlfn.IFS(OR(C24=1,C24="1"),188760, OR(C24=2,C24="2"),174390, OR(C24=3,C24="3"),126950, TRUE, ""),
-    A24="RICE LAND W/O IRRIGATION", _xlfn.IFS(OR(C24=1,C24="1"),82450, OR(C24=2,C24="2"),75070, OR(C24=3,C24="3"),52590, TRUE, ""),
-    A24="UPLAND RICE", 28540,
-    A24="ORCHARD", 44100,
-    A24="COGON LAND", 46460,
-    A24="NIPA LAND", 55070,
-    A24="FOREST LAND", 59660,
-    A24="FISHPOND", 218240,
-    TRUE, ""
-)</f>
-        <v/>
-      </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="43" t="str">
-        <f>IFERROR(MROUND(D24*E24,10),"")</f>
-        <v/>
-      </c>
-      <c r="H24" s="35"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="33"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="35"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="25"/>
       <c r="D25" s="29"/>
-      <c r="E25" s="48" t="str" cm="1">
-        <f t="array" ref="E25">_xlfn.IFS(
-    A25="COMMERCIAL", _xlfn.IFS(C25="C-1",1400, C25="C-2",1030, C25="C-3",850, C25="C-4",720, TRUE, ""),
-    A25="RESIDENTIAL", _xlfn.IFS(C25="R-1",760, C25="R-2",610, C25="R-3",470, C25="R-4",280, C25="R-5",200, TRUE, ""),
-    A25="COCONUT LAND", _xlfn.IFS(OR(C25=1,C25="1"),93830, OR(C25=2,C25="2"),84500, OR(C25=3,C25="3"),76130, TRUE, ""),
-    A25="RICE LAND W/ IRRIGATION", _xlfn.IFS(OR(C25=1,C25="1"),188760, OR(C25=2,C25="2"),174390, OR(C25=3,C25="3"),126950, TRUE, ""),
-    A25="RICE LAND W/O IRRIGATION", _xlfn.IFS(OR(C25=1,C25="1"),82450, OR(C25=2,C25="2"),75070, OR(C25=3,C25="3"),52590, TRUE, ""),
-    A25="UPLAND RICE", 28540,
-    A25="ORCHARD", 44100,
-    A25="COGON LAND", 46460,
-    A25="NIPA LAND", 55070,
-    A25="FOREST LAND", 59660,
-    A25="FISHPOND", 218240,
-    TRUE, ""
-)</f>
-        <v/>
-      </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="43" t="str">
-        <f>IFERROR(MROUND(D25*E25,10),"")</f>
-        <v/>
-      </c>
-      <c r="H25" s="35"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="33"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="43">
-        <f>SUM(G22:H25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="35"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="44" t="str">
+        <f>IF(SUM(G22:H25)=0, "", SUM(G22:H25))</f>
+        <v/>
+      </c>
+      <c r="H26" s="33"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="42" t="s">
+      <c r="B28" s="33"/>
+      <c r="C28" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="42" t="s">
+      <c r="D28" s="33"/>
+      <c r="E28" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="42" t="s">
+      <c r="F28" s="33"/>
+      <c r="G28" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="35"/>
+      <c r="H28" s="33"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="43">
-        <f t="array" ref="E29">_xlfn.IFS(
-    A29="COCO BRG.-1", 480,
-    A29="COCO BRG.-2", 420,
-    A29="COCO BRG.-3", 330,
-    A29="AVOCADO", 310,
-    A29="BANANA", 200,
-    A29="CACAO", 300,
-    A29="CALAMANSI", 360,
-    A29="CAMANSI", 420,
-    A29="CHICO", 630,
-    A29="COFFEE", 250,
-    A29="JACKFRUIT", 840,
-    A29="LANZONES", 460,
-    A29="MABOLO", 350,
-    A29="MANGO", 1750,
-    A29="ORANGE", 460,
-    A29="RAMBUTAN", 360,
-    A29="SANTOL", 620,
-    A29="SINEGUELAS", 310,
-    A29="STAR APPLE", 790,
-    A29="TAMARIND", 350,
-    A29="BAMBOO", 460,
-    A29="BURI", 410,
-    A29="NIPA", 240,
-    TRUE, 0
-)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="35"/>
-      <c r="G29" s="43">
-        <f t="array" ref="G29">_xlfn.IFS(
-    A29="COCO BRG.-1", 480,
-    A29="COCO BRG.-2", 420,
-    A29="COCO BRG.-3", 330,
-    A29="AVOCADO", 310,
-    A29="BANANA", 200,
-    A29="CACAO", 300,
-    A29="CALAMANSI", 360,
-    A29="CAMANSI", 420,
-    A29="CHICO", 630,
-    A29="COFFEE", 250,
-    A29="JACKFRUIT", 840,
-    A29="LANZONES", 460,
-    A29="MABOLO", 350,
-    A29="MANGO", 1750,
-    A29="ORANGE", 460,
-    A29="RAMBUTAN", 360,
-    A29="SANTOL", 620,
-    A29="SINEGUELAS", 310,
-    A29="STAR APPLE", 790,
-    A29="TAMARIND", 350,
-    A29="BAMBOO", 460,
-    A29="BURI", 410,
-    A29="NIPA", 240,
-    TRUE, 0
-) * C29</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="35"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="33"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="43">
-        <f t="array" ref="E30">_xlfn.IFS(
-    A30="COCO BRG.-1", 480,
-    A30="COCO BRG.-2", 420,
-    A30="COCO BRG.-3", 330,
-    A30="AVOCADO", 310,
-    A30="BANANA", 200,
-    A30="CACAO", 300,
-    A30="CALAMANSI", 360,
-    A30="CAMANSI", 420,
-    A30="CHICO", 630,
-    A30="COFFEE", 250,
-    A30="JACKFRUIT", 840,
-    A30="LANZONES", 460,
-    A30="MABOLO", 350,
-    A30="MANGO", 1750,
-    A30="ORANGE", 460,
-    A30="RAMBUTAN", 360,
-    A30="SANTOL", 620,
-    A30="SINEGUELAS", 310,
-    A30="STAR APPLE", 790,
-    A30="TAMARIND", 350,
-    A30="BAMBOO", 460,
-    A30="BURI", 410,
-    A30="NIPA", 240,
-    TRUE, 0
-) * C30</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="35"/>
-      <c r="G30" s="43">
-        <f>IFERROR(MROUND(C30*E30,10),"")</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="35"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="33"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="43">
-        <f t="array" ref="E31">_xlfn.IFS(
-    A31="COCO BRG.-1", 480,
-    A31="COCO BRG.-2", 420,
-    A31="COCO BRG.-3", 330,
-    A31="AVOCADO", 310,
-    A31="BANANA", 200,
-    A31="CACAO", 300,
-    A31="CALAMANSI", 360,
-    A31="CAMANSI", 420,
-    A31="CHICO", 630,
-    A31="COFFEE", 250,
-    A31="JACKFRUIT", 840,
-    A31="LANZONES", 460,
-    A31="MABOLO", 350,
-    A31="MANGO", 1750,
-    A31="ORANGE", 460,
-    A31="RAMBUTAN", 360,
-    A31="SANTOL", 620,
-    A31="SINEGUELAS", 310,
-    A31="STAR APPLE", 790,
-    A31="TAMARIND", 350,
-    A31="BAMBOO", 460,
-    A31="BURI", 410,
-    A31="NIPA", 240,
-    TRUE, 0
-) * C31</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="35"/>
-      <c r="G31" s="43">
-        <f>IFERROR(MROUND(C31*E31,10),"")</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="35"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="43">
-        <f t="array" ref="E32">_xlfn.IFS(
-    A32="COCO BRG.-1", 480,
-    A32="COCO BRG.-2", 420,
-    A32="COCO BRG.-3", 330,
-    A32="AVOCADO", 310,
-    A32="BANANA", 200,
-    A32="CACAO", 300,
-    A32="CALAMANSI", 360,
-    A32="CAMANSI", 420,
-    A32="CHICO", 630,
-    A32="COFFEE", 250,
-    A32="JACKFRUIT", 840,
-    A32="LANZONES", 460,
-    A32="MABOLO", 350,
-    A32="MANGO", 1750,
-    A32="ORANGE", 460,
-    A32="RAMBUTAN", 360,
-    A32="SANTOL", 620,
-    A32="SINEGUELAS", 310,
-    A32="STAR APPLE", 790,
-    A32="TAMARIND", 350,
-    A32="BAMBOO", 460,
-    A32="BURI", 410,
-    A32="NIPA", 240,
-    TRUE, 0
-) * C32</f>
-        <v>0</v>
-      </c>
-      <c r="F32" s="35"/>
-      <c r="G32" s="43">
-        <f>IFERROR(MROUND(C32*E32,10),"")</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="35"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="33"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="44">
-        <f>SUM(G29:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="35"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="78" t="str">
+        <f>IF(SUM(G29:H32)=0, "", SUM(G29:H32))</f>
+        <v/>
+      </c>
+      <c r="H33" s="33"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="70" t="s">
+      <c r="A34" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="35"/>
-      <c r="G35" s="42" t="s">
+      <c r="F35" s="33"/>
+      <c r="G35" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="35"/>
+      <c r="H35" s="33"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="str">
-        <f>G22</f>
-        <v/>
-      </c>
-      <c r="B36" s="35"/>
+      <c r="A36" s="44"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="23"/>
       <c r="D36" s="17"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="55" t="str">
-        <f>IFERROR(MROUND(A36*D36,10),"")</f>
-        <v/>
-      </c>
-      <c r="H36" s="35"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="33"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43" t="str">
-        <f>G23</f>
-        <v/>
-      </c>
-      <c r="B37" s="35"/>
+      <c r="A37" s="44"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="23"/>
       <c r="D37" s="17"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="55" t="str">
-        <f>IFERROR(MROUND(A37*D37,10),"")</f>
-        <v/>
-      </c>
-      <c r="H37" s="35"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="33"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="str">
-        <f>G24</f>
-        <v/>
-      </c>
-      <c r="B38" s="35"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="23"/>
       <c r="D38" s="17"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="55" t="str">
-        <f>IFERROR(MROUND(A38*D38,10),"")</f>
-        <v/>
-      </c>
-      <c r="H38" s="35"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="33"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="43">
-        <f>G33</f>
-        <v>0</v>
-      </c>
-      <c r="B39" s="35"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="23"/>
       <c r="D39" s="17"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="55">
-        <f>IFERROR(MROUND(A39*D39,10),"")</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="35"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="74"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="35"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="55">
-        <f>SUM(G36:H39)</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="35"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34" t="str">
+        <f>IF(SUM(G36:H39)=0, "", SUM(G36:H39))</f>
+        <v/>
+      </c>
+      <c r="H40" s="33"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1986,97 +1721,73 @@
       <c r="B42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="42" t="s">
+      <c r="C42" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="42" t="s">
+      <c r="D42" s="33"/>
+      <c r="E42" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="42" t="s">
+      <c r="F42" s="33"/>
+      <c r="G42" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="H42" s="35"/>
+      <c r="H42" s="33"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="25"/>
-      <c r="C43" s="55" t="str">
-        <f>G36</f>
-        <v/>
-      </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="55" t="e">
-        <f>MROUND(C43*E43,10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H43" s="35"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="33"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24"/>
       <c r="B44" s="25"/>
-      <c r="C44" s="55" t="str">
-        <f>G37</f>
-        <v/>
-      </c>
-      <c r="D44" s="35"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="55" t="e">
-        <f>MROUND(C44*E44,10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H44" s="35"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="33"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="26"/>
-      <c r="C45" s="55" t="str">
-        <f>G38</f>
-        <v/>
-      </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="55" t="e">
-        <f>MROUND(C45*E45,10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H45" s="35"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="33"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24"/>
       <c r="B46" s="27"/>
-      <c r="C46" s="55">
-        <f>G39</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="35"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="55">
-        <f>MROUND(C46*E46,10)</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="35"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="33"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="6"/>
       <c r="D47" s="15"/>
       <c r="E47" s="6"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="55" t="e">
-        <f>SUM(G43:H46)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H47" s="35"/>
+      <c r="G47" s="34" t="str">
+        <f>IF(SUM(G43:H46)=0, "", SUM(G43:H46))</f>
+        <v/>
+      </c>
+      <c r="H47" s="33"/>
     </row>
     <row r="48" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
@@ -2097,31 +1808,31 @@
       <c r="A50" s="9"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="67"/>
-      <c r="B51" s="39"/>
-      <c r="D51" s="70" t="s">
+      <c r="A51" s="56"/>
+      <c r="B51" s="52"/>
+      <c r="D51" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="71"/>
+      <c r="E51" s="42"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="70" t="s">
+      <c r="G51" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="71"/>
+      <c r="H51" s="42"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="74" t="s">
+      <c r="A52" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="D52" s="61" t="s">
+      <c r="B52" s="49"/>
+      <c r="D52" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="62"/>
-      <c r="G52" s="61" t="s">
+      <c r="E52" s="38"/>
+      <c r="G52" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="62"/>
+      <c r="H52" s="38"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
@@ -2130,15 +1841,15 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
-      <c r="D54" s="56" t="s">
+      <c r="D54" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="32"/>
+      <c r="E54" s="66"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="56" t="s">
+      <c r="G54" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="H54" s="32"/>
+      <c r="H54" s="66"/>
     </row>
     <row r="55" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
@@ -2152,75 +1863,75 @@
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
-      <c r="D56" s="70" t="s">
+      <c r="D56" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="E56" s="71"/>
+      <c r="E56" s="42"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="67" t="s">
+      <c r="G56" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="39"/>
+      <c r="H56" s="52"/>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="61" t="s">
+      <c r="D57" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="62"/>
+      <c r="E57" s="38"/>
       <c r="F57" s="11"/>
-      <c r="G57" s="68" t="s">
+      <c r="G57" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="H57" s="32"/>
+      <c r="H57" s="66"/>
     </row>
     <row r="58" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="73"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="57"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="38"/>
+      <c r="A60" s="70"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="49"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="50"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="58"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="59"/>
+      <c r="A61" s="71"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="72"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="58"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="59"/>
+      <c r="A62" s="71"/>
+      <c r="B62" s="66"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="66"/>
+      <c r="F62" s="66"/>
+      <c r="G62" s="66"/>
+      <c r="H62" s="72"/>
     </row>
     <row r="63" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="60"/>
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
+      <c r="A63" s="51"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="53"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
@@ -2237,51 +1948,155 @@
       <c r="A65" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="50"/>
-      <c r="C65" s="51"/>
+      <c r="B65" s="67"/>
+      <c r="C65" s="61"/>
       <c r="D65" s="20" t="s">
         <v>60</v>
       </c>
       <c r="E65" s="25"/>
-      <c r="F65" s="52" t="s">
+      <c r="F65" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="G65" s="51"/>
+      <c r="G65" s="61"/>
       <c r="H65" s="22"/>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="53" t="s">
+      <c r="A66" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="B66" s="63"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="53" t="s">
+      <c r="B66" s="62"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="E66" s="50"/>
-      <c r="F66" s="52" t="s">
+      <c r="E66" s="67"/>
+      <c r="F66" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="G66" s="51"/>
+      <c r="G66" s="61"/>
       <c r="H66" s="22"/>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="54"/>
-      <c r="B67" s="65"/>
-      <c r="C67" s="66"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="52" t="s">
+      <c r="A67" s="69"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="69"/>
+      <c r="E67" s="69"/>
+      <c r="F67" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="G67" s="51"/>
-      <c r="H67" s="22">
-        <f>SUM(H65:H66)</f>
-        <v>0</v>
+      <c r="G67" s="61"/>
+      <c r="H67" s="22" t="str">
+        <f>IF(SUM(H65:H66)=0, "", MROUND(SUM(H65:H66), 10))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B66:C67"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="A60:H63"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="B18:H18"/>
@@ -2306,110 +2121,6 @@
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="G38:H38"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="A60:H63"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="E40:F40"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>

</xml_diff>

<commit_message>
Edit Format in FAAS & UNIRRIG Excel
</commit_message>
<xml_diff>
--- a/backend/python/templates/FAAS_Template.xlsx
+++ b/backend/python/templates/FAAS_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Videos\FAAS SYSTEM\backend\python\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C41C3F-505F-46B1-963C-95842D6073AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3F824C-1A30-4F88-A8CB-5F8FCE57EF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,7 +224,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +280,21 @@
       <name val="Bahnschrift Condensed"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Bahnschrift Condensed"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -600,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -666,67 +681,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -736,10 +751,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,29 +770,50 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1194,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1212,28 +1251,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1256,463 +1295,463 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="46" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="59"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="40"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="77"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="46" t="s">
+      <c r="B10" s="84"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="40"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="47"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="83"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="33"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="36" t="s">
+      <c r="F21" s="35"/>
+      <c r="G21" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="33"/>
+      <c r="H21" s="35"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="33"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="35"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="26"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="33"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="35"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="26"/>
       <c r="D24" s="28"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="33"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="25"/>
       <c r="D25" s="29"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="33"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="35"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="33"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="44" t="str">
+      <c r="E26" s="41"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="42" t="str">
         <f>IF(SUM(G22:H25)=0, "", SUM(G22:H25))</f>
         <v/>
       </c>
-      <c r="H26" s="33"/>
+      <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="36" t="s">
+      <c r="B28" s="35"/>
+      <c r="C28" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="36" t="s">
+      <c r="D28" s="35"/>
+      <c r="E28" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="36" t="s">
+      <c r="F28" s="35"/>
+      <c r="G28" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="33"/>
+      <c r="H28" s="35"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="33"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="35"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="33"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="35"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="33"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="35"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="33"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="35"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="78" t="str">
+      <c r="B33" s="35"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="43" t="str">
         <f>IF(SUM(G29:H32)=0, "", SUM(G29:H32))</f>
         <v/>
       </c>
-      <c r="H33" s="33"/>
+      <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="33"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="36" t="s">
+      <c r="E35" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="33"/>
-      <c r="G35" s="36" t="s">
+      <c r="F35" s="35"/>
+      <c r="G35" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="33"/>
+      <c r="H35" s="35"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="33"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="23"/>
       <c r="D36" s="17"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="33"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="35"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="23"/>
       <c r="D37" s="17"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="33"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="35"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="23"/>
       <c r="D38" s="17"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="33"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="35"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="23"/>
       <c r="D39" s="17"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="74"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="33"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="34" t="str">
+      <c r="E40" s="41"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="54" t="str">
         <f>IF(SUM(G36:H39)=0, "", SUM(G36:H39))</f>
         <v/>
       </c>
-      <c r="H40" s="33"/>
+      <c r="H40" s="35"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="33"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1721,73 +1760,73 @@
       <c r="B42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="33"/>
-      <c r="E42" s="36" t="s">
+      <c r="D42" s="35"/>
+      <c r="E42" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="33"/>
-      <c r="G42" s="36" t="s">
+      <c r="F42" s="35"/>
+      <c r="G42" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="H42" s="33"/>
+      <c r="H42" s="35"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="25"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="33"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="35"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24"/>
       <c r="B44" s="25"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="33"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="35"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="26"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="33"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="35"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24"/>
       <c r="B46" s="27"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="33"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="35"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="33"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="6"/>
       <c r="D47" s="15"/>
       <c r="E47" s="6"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="34" t="str">
+      <c r="G47" s="54" t="str">
         <f>IF(SUM(G43:H46)=0, "", SUM(G43:H46))</f>
         <v/>
       </c>
-      <c r="H47" s="33"/>
+      <c r="H47" s="35"/>
     </row>
     <row r="48" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
@@ -1808,31 +1847,31 @@
       <c r="A50" s="9"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
-      <c r="B51" s="52"/>
-      <c r="D51" s="57" t="s">
+      <c r="A51" s="64"/>
+      <c r="B51" s="38"/>
+      <c r="D51" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="42"/>
+      <c r="E51" s="50"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="57" t="s">
+      <c r="G51" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="42"/>
+      <c r="H51" s="50"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="55" t="s">
+      <c r="A52" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="49"/>
-      <c r="D52" s="37" t="s">
+      <c r="B52" s="36"/>
+      <c r="D52" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="38"/>
-      <c r="G52" s="37" t="s">
+      <c r="E52" s="57"/>
+      <c r="G52" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="38"/>
+      <c r="H52" s="57"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
@@ -1841,15 +1880,15 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
-      <c r="D54" s="75" t="s">
+      <c r="D54" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="66"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="75" t="s">
+      <c r="G54" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="H54" s="66"/>
+      <c r="H54" s="32"/>
     </row>
     <row r="55" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
@@ -1863,75 +1902,75 @@
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
-      <c r="D56" s="57" t="s">
+      <c r="D56" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="E56" s="42"/>
+      <c r="E56" s="50"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="56" t="s">
+      <c r="G56" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="52"/>
+      <c r="H56" s="38"/>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="37" t="s">
+      <c r="D57" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="38"/>
+      <c r="E57" s="57"/>
       <c r="F57" s="11"/>
       <c r="G57" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="H57" s="66"/>
+      <c r="H57" s="32"/>
     </row>
     <row r="58" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="54"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
+      <c r="B59" s="74"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="70"/>
-      <c r="B60" s="49"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="49"/>
-      <c r="E60" s="49"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="50"/>
+      <c r="A60" s="69"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="71"/>
-      <c r="B61" s="66"/>
-      <c r="C61" s="66"/>
-      <c r="D61" s="66"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="66"/>
-      <c r="G61" s="66"/>
-      <c r="H61" s="72"/>
+      <c r="A61" s="70"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="71"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="71"/>
-      <c r="B62" s="66"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="66"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="66"/>
-      <c r="G62" s="66"/>
-      <c r="H62" s="72"/>
+      <c r="A62" s="70"/>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="71"/>
     </row>
     <row r="63" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="51"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="52"/>
-      <c r="H63" s="53"/>
+      <c r="A63" s="72"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="39"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
@@ -1948,44 +1987,44 @@
       <c r="A65" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="67"/>
-      <c r="C65" s="61"/>
+      <c r="B65" s="66"/>
+      <c r="C65" s="59"/>
       <c r="D65" s="20" t="s">
         <v>60</v>
       </c>
       <c r="E65" s="25"/>
-      <c r="F65" s="60" t="s">
+      <c r="F65" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="G65" s="61"/>
+      <c r="G65" s="59"/>
       <c r="H65" s="22"/>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="68" t="s">
+      <c r="A66" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="B66" s="62"/>
-      <c r="C66" s="63"/>
-      <c r="D66" s="68" t="s">
+      <c r="B66" s="60"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="E66" s="67"/>
-      <c r="F66" s="60" t="s">
+      <c r="E66" s="66"/>
+      <c r="F66" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="G66" s="61"/>
+      <c r="G66" s="59"/>
       <c r="H66" s="22"/>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="69"/>
-      <c r="B67" s="64"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="69"/>
-      <c r="E67" s="69"/>
-      <c r="F67" s="60" t="s">
+      <c r="A67" s="68"/>
+      <c r="B67" s="62"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="G67" s="61"/>
+      <c r="G67" s="59"/>
       <c r="H67" s="22" t="str">
         <f>IF(SUM(H65:H66)=0, "", MROUND(SUM(H65:H66), 10))</f>
         <v/>
@@ -1993,6 +2032,110 @@
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F10:H11"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B66:C67"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="A60:H63"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G40:H40"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B10:D11"/>
@@ -2017,110 +2160,6 @@
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="A60:H63"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F10:H11"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="G38:H38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>

</xml_diff>

<commit_message>
02-23-26 Tax Dec Finalization
</commit_message>
<xml_diff>
--- a/backend/python/templates/FAAS_Template.xlsx
+++ b/backend/python/templates/FAAS_Template.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Videos\FAAS SYSTEM\backend\python\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3F824C-1A30-4F88-A8CB-5F8FCE57EF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4185BC-251A-4217-B4E3-2F236BE268EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRINT" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PRINT!$A$1:$H$70</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>MUNICIPALITY OF BOAC</t>
   </si>
@@ -304,7 +307,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -608,6 +611,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -615,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -681,67 +695,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -755,9 +750,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -765,40 +769,39 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -814,6 +817,39 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1231,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:H11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1251,28 +1287,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1295,463 +1331,463 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="35"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="44" t="s">
+      <c r="B8" s="72"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="76"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="77"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="76"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="63"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="52"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="44" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="76"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="45"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="41" t="s">
+      <c r="F21" s="33"/>
+      <c r="G21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="35"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="35"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="26"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="35"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="33"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="26"/>
       <c r="D24" s="28"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="35"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="33"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="35"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="25"/>
       <c r="D25" s="29"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="35"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="33"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="42" t="str">
+      <c r="E26" s="36"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="45" t="str">
         <f>IF(SUM(G22:H25)=0, "", SUM(G22:H25))</f>
         <v/>
       </c>
-      <c r="H26" s="35"/>
+      <c r="H26" s="33"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="41" t="s">
+      <c r="B28" s="33"/>
+      <c r="C28" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="41" t="s">
+      <c r="D28" s="33"/>
+      <c r="E28" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="41" t="s">
+      <c r="F28" s="33"/>
+      <c r="G28" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="35"/>
+      <c r="H28" s="33"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="35"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="33"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="35"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="33"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="35"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="33"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="35"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="33"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="43" t="str">
+      <c r="B33" s="33"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="84" t="str">
         <f>IF(SUM(G29:H32)=0, "", SUM(G29:H32))</f>
         <v/>
       </c>
-      <c r="H33" s="35"/>
+      <c r="H33" s="33"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="s">
+      <c r="A34" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="41" t="s">
+      <c r="E35" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="35"/>
-      <c r="G35" s="41" t="s">
+      <c r="F35" s="33"/>
+      <c r="G35" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="35"/>
+      <c r="H35" s="33"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="35"/>
+      <c r="A36" s="45"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="23"/>
       <c r="D36" s="17"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="35"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="33"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="23"/>
       <c r="D37" s="17"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="35"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="33"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="45"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="23"/>
       <c r="D38" s="17"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="35"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="33"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="45"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="23"/>
       <c r="D39" s="17"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="53"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="67"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="35"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="54" t="str">
+      <c r="E40" s="36"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34" t="str">
         <f>IF(SUM(G36:H39)=0, "", SUM(G36:H39))</f>
         <v/>
       </c>
-      <c r="H40" s="35"/>
+      <c r="H40" s="33"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1760,73 +1796,73 @@
       <c r="B42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="41" t="s">
+      <c r="D42" s="33"/>
+      <c r="E42" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="41" t="s">
+      <c r="F42" s="33"/>
+      <c r="G42" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="H42" s="35"/>
+      <c r="H42" s="33"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="25"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="35"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="33"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24"/>
       <c r="B44" s="25"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="35"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="33"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="26"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="35"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="33"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="24"/>
       <c r="B46" s="27"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="35"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="33"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="6"/>
       <c r="D47" s="15"/>
       <c r="E47" s="6"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="54" t="str">
+      <c r="G47" s="34" t="str">
         <f>IF(SUM(G43:H46)=0, "", SUM(G43:H46))</f>
         <v/>
       </c>
-      <c r="H47" s="35"/>
+      <c r="H47" s="33"/>
     </row>
     <row r="48" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
@@ -1847,31 +1883,31 @@
       <c r="A50" s="9"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="64"/>
-      <c r="B51" s="38"/>
-      <c r="D51" s="49" t="s">
+      <c r="A51" s="53"/>
+      <c r="B51" s="54"/>
+      <c r="D51" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="50"/>
+      <c r="E51" s="59"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="49" t="s">
+      <c r="G51" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="50"/>
+      <c r="H51" s="59"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="75" t="s">
+      <c r="A52" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="D52" s="56" t="s">
+      <c r="B52" s="65"/>
+      <c r="D52" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="57"/>
-      <c r="G52" s="56" t="s">
+      <c r="E52" s="38"/>
+      <c r="G52" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="57"/>
+      <c r="H52" s="38"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
@@ -1880,15 +1916,15 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
-      <c r="D54" s="55" t="s">
+      <c r="D54" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="32"/>
+      <c r="E54" s="56"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="55" t="s">
+      <c r="G54" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="H54" s="32"/>
+      <c r="H54" s="56"/>
     </row>
     <row r="55" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
@@ -1902,136 +1938,273 @@
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
-      <c r="D56" s="49" t="s">
+      <c r="D56" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="E56" s="50"/>
+      <c r="E56" s="59"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="64" t="s">
+      <c r="G56" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="38"/>
+      <c r="H56" s="54"/>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="56" t="s">
+      <c r="D57" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="57"/>
+      <c r="E57" s="38"/>
       <c r="F57" s="11"/>
-      <c r="G57" s="65" t="s">
+      <c r="G57" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="H57" s="32"/>
+      <c r="H57" s="56"/>
     </row>
     <row r="58" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="74"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="69"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="37"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="70"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="71"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="70"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="71"/>
-    </row>
-    <row r="63" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="72"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="39"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="12" t="s">
+      <c r="A60" s="86"/>
+      <c r="B60" s="87"/>
+      <c r="C60" s="87"/>
+      <c r="D60" s="87"/>
+      <c r="E60" s="87"/>
+      <c r="F60" s="87"/>
+      <c r="G60" s="87"/>
+      <c r="H60" s="88"/>
+    </row>
+    <row r="61" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="89"/>
+      <c r="B61" s="90"/>
+      <c r="C61" s="90"/>
+      <c r="D61" s="90"/>
+      <c r="E61" s="90"/>
+      <c r="F61" s="90"/>
+      <c r="G61" s="90"/>
+      <c r="H61" s="91"/>
+    </row>
+    <row r="62" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="92"/>
+      <c r="B62" s="93"/>
+      <c r="C62" s="93"/>
+      <c r="D62" s="93"/>
+      <c r="E62" s="93"/>
+      <c r="F62" s="93"/>
+      <c r="G62" s="93"/>
+      <c r="H62" s="94"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="H64" s="16"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="H63" s="16"/>
+    </row>
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="60"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" s="25"/>
+      <c r="F64" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G64" s="48"/>
+      <c r="H64" s="22"/>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65" s="49"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="60"/>
+      <c r="F65" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="G65" s="48"/>
+      <c r="H65" s="22"/>
+    </row>
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="62"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G66" s="48"/>
+      <c r="H66" s="22" t="str">
+        <f>IF(SUM(H64:H65)=0, "", MROUND(SUM(H64:H65), 10))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="66"/>
-      <c r="C65" s="59"/>
-      <c r="D65" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E65" s="25"/>
-      <c r="F65" s="58" t="s">
+      <c r="B68" s="60"/>
+      <c r="C68" s="48"/>
+      <c r="F68" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="G65" s="59"/>
-      <c r="H65" s="22"/>
-    </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="67" t="s">
+      <c r="G68" s="48"/>
+      <c r="H68" s="22"/>
+    </row>
+    <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="B66" s="60"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="E66" s="66"/>
-      <c r="F66" s="58" t="s">
+      <c r="B69" s="49"/>
+      <c r="C69" s="50"/>
+      <c r="F69" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="G66" s="59"/>
-      <c r="H66" s="22"/>
-    </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="68"/>
-      <c r="B67" s="62"/>
-      <c r="C67" s="63"/>
-      <c r="D67" s="68"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="58" t="s">
+      <c r="G69" s="48"/>
+      <c r="H69" s="22"/>
+    </row>
+    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="62"/>
+      <c r="B70" s="51"/>
+      <c r="C70" s="52"/>
+      <c r="F70" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="G67" s="59"/>
-      <c r="H67" s="22" t="str">
-        <f>IF(SUM(H65:H66)=0, "", MROUND(SUM(H65:H66), 10))</f>
+      <c r="G70" s="48"/>
+      <c r="H70" s="22" t="str">
+        <f>IF(SUM(H68:H69)=0, "", MROUND(SUM(H68:H69), 10))</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="128">
+  <mergeCells count="134">
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="B65:C66"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A60:H62"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="B18:H18"/>
@@ -2056,110 +2229,6 @@
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="G38:H38"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="A60:H63"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="E40:F40"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>

</xml_diff>

<commit_message>
02-27-26 TDC Back page TCT
</commit_message>
<xml_diff>
--- a/backend/python/templates/FAAS_Template.xlsx
+++ b/backend/python/templates/FAAS_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Videos\FAAS SYSTEM\backend\python\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8142F5E6-6507-42F6-ACD1-C58646353C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A1DEC-DF51-4802-B913-1F3BB3734090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -674,11 +674,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -688,100 +686,118 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -810,51 +826,37 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1278,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1296,28 +1298,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1340,210 +1342,210 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="38"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="39"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="48" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="69"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="73"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="55"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="48" t="s">
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="69"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="96"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="97"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="99"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="96"/>
       <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="38"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="39"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="39"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="39"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="39"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="38"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
@@ -1553,169 +1555,169 @@
       <c r="E21" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="38"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="38"/>
+      <c r="H21" s="39"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="38"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="38"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="39"/>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="26"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="14"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="38"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="39"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="14"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="38"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="39"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="14"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="38"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="39"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="38"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="45"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="46" t="str">
+      <c r="F26" s="39"/>
+      <c r="G26" s="42" t="str">
         <f>IF(SUM(G22:H25)=0, "", SUM(G22:H25))</f>
         <v/>
       </c>
-      <c r="H26" s="38"/>
+      <c r="H26" s="39"/>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="39"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="39"/>
       <c r="C28" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="38"/>
+      <c r="D28" s="39"/>
       <c r="E28" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="38"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="38"/>
+      <c r="H28" s="39"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="38"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="39"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="45"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="39"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="45"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="39"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="45"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="39"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="38"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="45"/>
-      <c r="D33" s="38"/>
+      <c r="D33" s="39"/>
       <c r="E33" s="45"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="47" t="str">
+      <c r="F33" s="39"/>
+      <c r="G33" s="42" t="str">
         <f>IF(SUM(G29:H32)=0, "", SUM(G29:H32))</f>
         <v/>
       </c>
-      <c r="H33" s="38"/>
+      <c r="H33" s="39"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="5" t="s">
         <v>31</v>
       </c>
@@ -1725,78 +1727,80 @@
       <c r="E35" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="38"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="38"/>
+      <c r="H35" s="39"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="23"/>
+      <c r="A36" s="42">
+        <v>1212</v>
+      </c>
+      <c r="B36" s="39"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="17"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="38"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="39"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="23"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="17"/>
       <c r="E37" s="45"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="38"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="39"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="23"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="17"/>
       <c r="E38" s="45"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="38"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="39"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="23"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="17"/>
       <c r="E39" s="45"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="86"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="76"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="45"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="61" t="str">
+      <c r="F40" s="39"/>
+      <c r="G40" s="42" t="str">
         <f>IF(SUM(G36:H39)=0, "", SUM(G36:H39))</f>
         <v/>
       </c>
-      <c r="H40" s="38"/>
+      <c r="H40" s="39"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="38"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="39"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
@@ -1808,70 +1812,70 @@
       <c r="C42" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="38"/>
+      <c r="D42" s="39"/>
       <c r="E42" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="38"/>
+      <c r="F42" s="39"/>
       <c r="G42" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H42" s="38"/>
+      <c r="H42" s="39"/>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="84"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="38"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="39"/>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="38"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="39"/>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="38"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="39"/>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="84"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="38"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="39"/>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="38"/>
+      <c r="B47" s="39"/>
       <c r="C47" s="6"/>
       <c r="D47" s="15"/>
       <c r="E47" s="6"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="61" t="str">
+      <c r="G47" s="42" t="str">
         <f>IF(SUM(G43:H46)=0, "", SUM(G43:H46))</f>
         <v/>
       </c>
-      <c r="H47" s="38"/>
+      <c r="H47" s="39"/>
     </row>
     <row r="48" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="8"/>
@@ -1892,31 +1896,31 @@
       <c r="A50" s="9"/>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="74"/>
-      <c r="B51" s="60"/>
-      <c r="D51" s="67" t="s">
+      <c r="A51" s="56"/>
+      <c r="B51" s="57"/>
+      <c r="D51" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="68"/>
+      <c r="E51" s="47"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="67" t="s">
+      <c r="G51" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="68"/>
+      <c r="H51" s="47"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="93" t="s">
+      <c r="A52" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="58"/>
-      <c r="D52" s="87" t="s">
+      <c r="B52" s="65"/>
+      <c r="D52" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="70"/>
-      <c r="G52" s="87" t="s">
+      <c r="E52" s="44"/>
+      <c r="G52" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="70"/>
+      <c r="H52" s="44"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
@@ -1925,15 +1929,15 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
-      <c r="D54" s="94" t="s">
+      <c r="D54" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="35"/>
+      <c r="E54" s="49"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="94" t="s">
+      <c r="G54" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="H54" s="35"/>
+      <c r="H54" s="49"/>
     </row>
     <row r="55" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="9"/>
@@ -1947,65 +1951,65 @@
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
-      <c r="D56" s="67" t="s">
+      <c r="D56" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E56" s="68"/>
+      <c r="E56" s="47"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="74" t="s">
+      <c r="G56" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="60"/>
+      <c r="H56" s="57"/>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="87" t="s">
+      <c r="D57" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="70"/>
+      <c r="E57" s="44"/>
       <c r="F57" s="11"/>
-      <c r="G57" s="90" t="s">
+      <c r="G57" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="H57" s="35"/>
+      <c r="H57" s="49"/>
     </row>
     <row r="58" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="92"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
     </row>
     <row r="60" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="75"/>
-      <c r="B60" s="76"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="76"/>
-      <c r="G60" s="76"/>
-      <c r="H60" s="77"/>
+      <c r="A60" s="79"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="80"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="81"/>
     </row>
     <row r="61" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="78"/>
-      <c r="B61" s="79"/>
-      <c r="C61" s="79"/>
-      <c r="D61" s="79"/>
-      <c r="E61" s="79"/>
-      <c r="F61" s="79"/>
-      <c r="G61" s="79"/>
-      <c r="H61" s="80"/>
+      <c r="A61" s="82"/>
+      <c r="B61" s="83"/>
+      <c r="C61" s="83"/>
+      <c r="D61" s="83"/>
+      <c r="E61" s="83"/>
+      <c r="F61" s="83"/>
+      <c r="G61" s="83"/>
+      <c r="H61" s="84"/>
     </row>
     <row r="62" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="81"/>
-      <c r="B62" s="82"/>
-      <c r="C62" s="82"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="82"/>
-      <c r="F62" s="82"/>
-      <c r="G62" s="82"/>
-      <c r="H62" s="83"/>
+      <c r="A62" s="85"/>
+      <c r="B62" s="86"/>
+      <c r="C62" s="86"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="86"/>
+      <c r="F62" s="86"/>
+      <c r="G62" s="86"/>
+      <c r="H62" s="87"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
@@ -2022,94 +2026,207 @@
       <c r="A64" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B64" s="91"/>
-      <c r="C64" s="54"/>
+      <c r="B64" s="60"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E64" s="25"/>
-      <c r="F64" s="53" t="s">
+      <c r="E64" s="23"/>
+      <c r="F64" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="G64" s="54"/>
-      <c r="H64" s="22"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="31"/>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="55" t="s">
+      <c r="A65" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="88"/>
-      <c r="C65" s="89"/>
-      <c r="D65" s="55" t="s">
+      <c r="B65" s="52"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="E65" s="91"/>
-      <c r="F65" s="53" t="s">
+      <c r="E65" s="60"/>
+      <c r="F65" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="G65" s="54"/>
-      <c r="H65" s="22"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="31"/>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="56"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="73"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="53" t="s">
+      <c r="A66" s="62"/>
+      <c r="B66" s="54"/>
+      <c r="C66" s="55"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="G66" s="54"/>
-      <c r="H66" s="22" t="str">
+      <c r="G66" s="51"/>
+      <c r="H66" s="31" t="str">
         <f>IF(SUM(H64:H65)=0, "", MROUND(SUM(H64:H65), 10))</f>
         <v/>
       </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H67" s="31"/>
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B68" s="52"/>
-      <c r="C68" s="37"/>
+      <c r="B68" s="77"/>
+      <c r="C68" s="41"/>
       <c r="D68" s="6"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="53" t="s">
+      <c r="E68" s="28"/>
+      <c r="F68" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="G68" s="54"/>
-      <c r="H68" s="22"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="31"/>
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="55" t="s">
+      <c r="A69" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="B69" s="57"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="53" t="s">
+      <c r="B69" s="78"/>
+      <c r="C69" s="65"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="G69" s="54"/>
-      <c r="H69" s="22"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="31"/>
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="56"/>
-      <c r="B70" s="59"/>
-      <c r="C70" s="60"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="53" t="s">
+      <c r="A70" s="62"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="57"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="27"/>
+      <c r="F70" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="G70" s="54"/>
-      <c r="H70" s="22" t="str">
+      <c r="G70" s="51"/>
+      <c r="H70" s="31" t="str">
         <f>IF(SUM(H68:H69)=0, "", MROUND(SUM(H68:H69), 10))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="134">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B10:D11"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A60:H62"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="F8:H9"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="B65:C66"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G35:H35"/>
     <mergeCell ref="F10:H11"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>
@@ -2134,116 +2251,6 @@
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="F14:H14"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="F8:H9"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A60:H62"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B10:D11"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <conditionalFormatting sqref="D22:D25">
     <cfRule type="expression" dxfId="0" priority="3">

</xml_diff>